<commit_message>
Updating rmd Cleaning up quality criteria More analyses Making qualinprogress work as pdf creator of images
</commit_message>
<xml_diff>
--- a/reports/quality_scores_vals.xlsx
+++ b/reports/quality_scores_vals.xlsx
@@ -12,213 +12,405 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
   <si>
     <t xml:space="preserve">Study</t>
   </si>
   <si>
-    <t xml:space="preserve">JBI1_inclusion_criteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JBI2_subjects_setting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JBI3_exposure_measurement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JBI5_confounds_identified</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JBI6_confounds_addressed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JBI7_outcomes_measured</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JBI8_appropriate_statistics</t>
+    <t xml:space="preserve">unique_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J8</t>
   </si>
   <si>
     <t xml:space="preserve">screen</t>
   </si>
   <si>
-    <t xml:space="preserve">Overall</t>
-  </si>
-  <si>
     <t xml:space="preserve">Weight</t>
   </si>
   <si>
     <t xml:space="preserve">quality_quant</t>
   </si>
   <si>
+    <t xml:space="preserve">toggle</t>
+  </si>
+  <si>
     <t xml:space="preserve">Weiner et al. (2006)</t>
   </si>
   <si>
+    <t xml:space="preserve">WEI184</t>
+  </si>
+  <si>
     <t xml:space="preserve">MMSE</t>
   </si>
   <si>
-    <t xml:space="preserve"/>
+    <t xml:space="preserve">0</t>
   </si>
   <si>
     <t xml:space="preserve">Al-Malki et al. (2020)</t>
   </si>
   <si>
+    <t xml:space="preserve">ALM009</t>
+  </si>
+  <si>
     <t xml:space="preserve">MoCA</t>
   </si>
   <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cardoso et al. (2021)</t>
   </si>
   <si>
+    <t xml:space="preserve">APA016</t>
+  </si>
+  <si>
     <t xml:space="preserve">Barceló-Martinez et al. (2018)</t>
   </si>
   <si>
+    <t xml:space="preserve">BAR026</t>
+  </si>
+  <si>
     <t xml:space="preserve">Boldt et al. (2020)</t>
   </si>
   <si>
+    <t xml:space="preserve">BOL034</t>
+  </si>
+  <si>
     <t xml:space="preserve">Borg et al. (2015)</t>
   </si>
   <si>
+    <t xml:space="preserve">BOR37</t>
+  </si>
+  <si>
     <t xml:space="preserve">Buckalew et al. (2008)</t>
   </si>
   <si>
+    <t xml:space="preserve">BUC047</t>
+  </si>
+  <si>
     <t xml:space="preserve">Can et al. (2012)</t>
   </si>
   <si>
-    <t xml:space="preserve">Chen et al. (2017)</t>
+    <t xml:space="preserve">CAN053</t>
   </si>
   <si>
     <t xml:space="preserve">Chen et al. (2016)</t>
   </si>
   <si>
+    <t xml:space="preserve">CHE063-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHE063-B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coelho Rebelo Maia (2012)</t>
   </si>
   <si>
+    <t xml:space="preserve">COE069</t>
+  </si>
+  <si>
     <t xml:space="preserve">Corti et al. (2021)</t>
   </si>
   <si>
+    <t xml:space="preserve">COR070</t>
+  </si>
+  <si>
     <t xml:space="preserve">HVLT</t>
   </si>
   <si>
     <t xml:space="preserve">Demirci &amp; Savas (2002)</t>
   </si>
   <si>
+    <t xml:space="preserve">DEM077</t>
+  </si>
+  <si>
     <t xml:space="preserve">Di Carlo et al. (2021)</t>
   </si>
   <si>
+    <t xml:space="preserve">DIC079</t>
+  </si>
+  <si>
     <t xml:space="preserve">El-Shafey et al. (2012)</t>
   </si>
   <si>
+    <t xml:space="preserve">ELS083</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fayed et al. (2012)</t>
   </si>
   <si>
+    <t xml:space="preserve">FAY089-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAY089-B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fayed et al. (2017)</t>
   </si>
   <si>
+    <t xml:space="preserve">FAY090</t>
+  </si>
+  <si>
     <t xml:space="preserve">Feng et al. (2020)</t>
   </si>
   <si>
+    <t xml:space="preserve">FEN092</t>
+  </si>
+  <si>
     <t xml:space="preserve">Foss et al. (2016)</t>
   </si>
   <si>
+    <t xml:space="preserve">FOS095</t>
+  </si>
+  <si>
     <t xml:space="preserve">Garcia et al. (2021)</t>
   </si>
   <si>
+    <t xml:space="preserve">GAR096</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gwinnutt et al. (2021)</t>
   </si>
   <si>
+    <t xml:space="preserve">GWI102</t>
+  </si>
+  <si>
     <t xml:space="preserve">ACE</t>
   </si>
   <si>
     <t xml:space="preserve">Karp et al. (2008)</t>
   </si>
   <si>
+    <t xml:space="preserve">KAR113</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kim &amp; Buschmann (2006)</t>
   </si>
   <si>
+    <t xml:space="preserve">KIM114</t>
+  </si>
+  <si>
     <t xml:space="preserve">Li et al. (2018)</t>
   </si>
   <si>
+    <t xml:space="preserve">LI_120</t>
+  </si>
+  <si>
     <t xml:space="preserve">Liao et al. (2018)</t>
   </si>
   <si>
+    <t xml:space="preserve">LIA121-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIA121-B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ma et al. (2017)</t>
   </si>
   <si>
+    <t xml:space="preserve">MA_125</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ojeda et al. (2016)</t>
   </si>
   <si>
+    <t xml:space="preserve">OJE134-NP-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OJE134-MSK-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OJE134-FM-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OJE134-NP-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OJE134-MSK-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OJE134-FM-B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oláh et al. (2020)</t>
   </si>
   <si>
+    <t xml:space="preserve">OLÁ136</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oosterman et al. (2011)</t>
   </si>
   <si>
+    <t xml:space="preserve">OOS137</t>
+  </si>
+  <si>
     <t xml:space="preserve">Petersen et al. (2015)</t>
   </si>
   <si>
+    <t xml:space="preserve">PET143</t>
+  </si>
+  <si>
     <t xml:space="preserve">Qu et al. (2018)</t>
   </si>
   <si>
+    <t xml:space="preserve">QU_144</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ruscheweyh et al. (2018)</t>
   </si>
   <si>
+    <t xml:space="preserve">RUS149</t>
+  </si>
+  <si>
     <t xml:space="preserve">Seo et al. (2017)</t>
   </si>
   <si>
+    <t xml:space="preserve">SEO156</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shehata et al. (2010)</t>
   </si>
   <si>
+    <t xml:space="preserve">SHE158</t>
+  </si>
+  <si>
     <t xml:space="preserve">Terassi et al. (2021)</t>
   </si>
   <si>
+    <t xml:space="preserve">TER167-COMB</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tiwari et al. (2021)</t>
   </si>
   <si>
+    <t xml:space="preserve">TIW171</t>
+  </si>
+  <si>
     <t xml:space="preserve">Torkamani et al. (2015)</t>
   </si>
   <si>
+    <t xml:space="preserve">TOR173</t>
+  </si>
+  <si>
     <t xml:space="preserve">Veldhuijzen et al. (2012)</t>
   </si>
   <si>
+    <t xml:space="preserve">VEL178</t>
+  </si>
+  <si>
     <t xml:space="preserve">R. Wang et al. (2014)</t>
   </si>
   <si>
+    <t xml:space="preserve">WAN182-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WAN182-B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y. Wang et al. (2014)</t>
   </si>
   <si>
+    <t xml:space="preserve">WAN183</t>
+  </si>
+  <si>
     <t xml:space="preserve">Canfora et al. (2021)</t>
   </si>
   <si>
+    <t xml:space="preserve">CAN194</t>
+  </si>
+  <si>
     <t xml:space="preserve">Segura-Jiménez et al. (2015)</t>
   </si>
   <si>
+    <t xml:space="preserve">SEG999</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mednieks et al. (2021)</t>
   </si>
   <si>
+    <t xml:space="preserve">MED128</t>
+  </si>
+  <si>
     <t xml:space="preserve">Xiang et al. (2021)</t>
   </si>
   <si>
+    <t xml:space="preserve">XIA186</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maneeton et al. (2010)</t>
   </si>
   <si>
+    <t xml:space="preserve">MAN998</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hamed et al. (2012)</t>
   </si>
   <si>
+    <t xml:space="preserve">HAM196</t>
+  </si>
+  <si>
     <t xml:space="preserve">Baptista et al. (2017)</t>
   </si>
   <si>
+    <t xml:space="preserve">BAP992</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vitturi et al. (2019)</t>
   </si>
   <si>
+    <t xml:space="preserve">VIT197-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIT197-B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Peterson et al. (2018)</t>
   </si>
   <si>
+    <t xml:space="preserve">PET994-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PET994-B</t>
+  </si>
+  <si>
     <t xml:space="preserve">Güzel et al. (2018)</t>
   </si>
   <si>
+    <t xml:space="preserve">GUZ995</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kotb et al. (2019)</t>
   </si>
   <si>
+    <t xml:space="preserve">KOT997</t>
+  </si>
+  <si>
     <t xml:space="preserve">Petra et al. (2020)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PET991</t>
   </si>
 </sst>
 </file>
@@ -587,788 +779,886 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
       </c>
       <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
         <v>14</v>
       </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>4</v>
+      <c r="M2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
-        <v>16</v>
+      <c r="I3" t="n">
+        <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K3" t="n">
         <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K4" t="n">
         <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="M4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5"/>
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
       </c>
-      <c r="I5" t="s">
-        <v>13</v>
+      <c r="I5" t="n">
+        <v>3</v>
       </c>
       <c r="J5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K5" t="n">
         <v>1</v>
       </c>
       <c r="L5" t="n">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="M5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
         <v>19</v>
       </c>
-      <c r="B6"/>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6"/>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
         <v>14</v>
       </c>
-      <c r="K6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" t="n">
-        <v>3</v>
+      <c r="M6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7"/>
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
       <c r="H7" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="I7" t="n">
+        <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K7" t="n">
         <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="M7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8"/>
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
       <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K8" t="n">
         <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c r="M8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" t="n">
         <v>22</v>
       </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" t="n">
-        <v>1</v>
-      </c>
-      <c r="L9" t="n">
-        <v>8</v>
+      <c r="M9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
         <v>1</v>
       </c>
-      <c r="I10" t="s">
-        <v>16</v>
+      <c r="I10" t="n">
+        <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K10" t="n">
         <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="M10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
       </c>
-      <c r="I11" t="s">
-        <v>16</v>
+      <c r="I11" t="n">
+        <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="M11" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12"/>
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H12" t="n">
         <v>1</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" t="n">
+        <v>3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" t="n">
         <v>13</v>
       </c>
-      <c r="J12" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" t="n">
-        <v>3</v>
+      <c r="M12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
       </c>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13" t="s">
-        <v>27</v>
+      <c r="G13" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2</v>
       </c>
       <c r="J13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" t="n">
         <v>14</v>
       </c>
-      <c r="K13" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" t="n">
-        <v>3</v>
+      <c r="M13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14"/>
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
       </c>
-      <c r="I14" t="s">
-        <v>13</v>
+      <c r="I14" t="n">
+        <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K14" t="n">
         <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="M14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="I15" t="n">
+        <v>3</v>
       </c>
       <c r="J15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K15" t="n">
         <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="M15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16"/>
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
       <c r="C16" t="n">
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
         <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H16" t="n">
         <v>1</v>
       </c>
-      <c r="I16" t="s">
-        <v>16</v>
+      <c r="I16" t="n">
+        <v>3</v>
       </c>
       <c r="J16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" t="n">
         <v>14</v>
       </c>
-      <c r="K16" t="n">
-        <v>1</v>
-      </c>
-      <c r="L16" t="n">
-        <v>4</v>
+      <c r="M16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
         <v>1</v>
       </c>
-      <c r="I17" t="s">
-        <v>13</v>
+      <c r="I17" t="n">
+        <v>3</v>
       </c>
       <c r="J17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K17" t="n">
         <v>1</v>
       </c>
       <c r="L17" t="n">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="M17" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18"/>
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3</v>
+      </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" t="n">
         <v>1</v>
       </c>
-      <c r="I18" t="s">
-        <v>13</v>
+      <c r="I18" t="n">
+        <v>3</v>
       </c>
       <c r="J18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K18" t="n">
         <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="M18" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" t="n">
+        <v>3</v>
+      </c>
+      <c r="J19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" t="n">
+        <v>1</v>
+      </c>
+      <c r="L19" t="n">
         <v>13</v>
       </c>
-      <c r="J19" t="s">
-        <v>14</v>
-      </c>
-      <c r="K19" t="n">
-        <v>1</v>
-      </c>
-      <c r="L19" t="n">
-        <v>1</v>
+      <c r="M19" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F20" t="n">
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
         <v>1</v>
       </c>
-      <c r="I20" t="s">
-        <v>16</v>
+      <c r="I20" t="n">
+        <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K20" t="n">
         <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="M20" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21"/>
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
+      </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
         <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H21" t="n">
         <v>1</v>
       </c>
-      <c r="I21" t="s">
-        <v>16</v>
+      <c r="I21" t="n">
+        <v>3</v>
       </c>
       <c r="J21" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K21" t="n">
         <v>1</v>
       </c>
       <c r="L21" t="n">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="M21" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" t="n">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H22" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" t="s">
-        <v>37</v>
+        <v>3</v>
+      </c>
+      <c r="I22" t="n">
+        <v>3</v>
       </c>
       <c r="J22" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K22" t="n">
         <v>1</v>
       </c>
       <c r="L22" t="n">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="M22" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" t="n">
-        <v>1</v>
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
-      </c>
-      <c r="D23"/>
+        <v>3</v>
+      </c>
+      <c r="D23" t="n">
+        <v>3</v>
+      </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
         <v>1</v>
@@ -1377,220 +1667,242 @@
         <v>1</v>
       </c>
       <c r="H23" t="n">
-        <v>1</v>
-      </c>
-      <c r="I23" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="I23" t="n">
+        <v>1</v>
       </c>
       <c r="J23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K23" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" t="n">
         <v>14</v>
       </c>
-      <c r="K23" t="n">
-        <v>1</v>
-      </c>
-      <c r="L23" t="n">
-        <v>6</v>
+      <c r="M23" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" t="n">
-        <v>1</v>
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
-      </c>
-      <c r="H24"/>
-      <c r="I24" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="H24" t="n">
+        <v>3</v>
+      </c>
+      <c r="I24" t="n">
+        <v>3</v>
       </c>
       <c r="J24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K24" t="n">
         <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>4</v>
+        <v>19</v>
+      </c>
+      <c r="M24" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" t="n">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>1</v>
-      </c>
-      <c r="I25" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="I25" t="n">
+        <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K25" t="n">
         <v>1</v>
       </c>
       <c r="L25" t="n">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="M25" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" t="n">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
       </c>
       <c r="C26" t="n">
         <v>1</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" t="n">
         <v>1</v>
       </c>
-      <c r="I26" t="s">
-        <v>16</v>
+      <c r="I26" t="n">
+        <v>3</v>
       </c>
       <c r="J26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K26" t="n">
         <v>1</v>
       </c>
       <c r="L26" t="n">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="M26" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" t="n">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" t="n">
         <v>1</v>
       </c>
-      <c r="I27" t="s">
-        <v>16</v>
+      <c r="I27" t="n">
+        <v>3</v>
       </c>
       <c r="J27" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L27" t="n">
         <v>14</v>
       </c>
-      <c r="K27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L27" t="n">
-        <v>3</v>
+      <c r="M27" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" t="n">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="B28" t="s">
+        <v>69</v>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E28" t="n">
         <v>1</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" t="n">
         <v>1</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="I28" t="n">
+        <v>3</v>
       </c>
       <c r="J28" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" t="n">
+        <v>1</v>
+      </c>
+      <c r="L28" t="n">
         <v>14</v>
       </c>
-      <c r="K28" t="n">
-        <v>1</v>
-      </c>
-      <c r="L28" t="n">
-        <v>5</v>
+      <c r="M28" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" t="n">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
+        <v>71</v>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29"/>
+        <v>3</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
       <c r="E29" t="n">
         <v>1</v>
       </c>
@@ -1598,441 +1910,493 @@
         <v>1</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" t="n">
         <v>1</v>
       </c>
-      <c r="I29" t="s">
-        <v>16</v>
+      <c r="I29" t="n">
+        <v>3</v>
       </c>
       <c r="J29" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K29" t="n">
         <v>1</v>
       </c>
       <c r="L29" t="n">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="M29" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30"/>
+        <v>72</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
+      </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
-      </c>
-      <c r="I30" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K30" t="n">
         <v>1</v>
       </c>
       <c r="L30" t="n">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="M30" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31"/>
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>74</v>
+      </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E31" t="n">
         <v>1</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G31" t="n">
         <v>1</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="I31" t="n">
+        <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K31" t="n">
         <v>1</v>
       </c>
       <c r="L31" t="n">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="M31" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" t="n">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="B32" t="s">
+        <v>75</v>
       </c>
       <c r="C32" t="n">
-        <v>1</v>
-      </c>
-      <c r="D32"/>
+        <v>3</v>
+      </c>
+      <c r="D32" t="n">
+        <v>3</v>
+      </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32" t="n">
-        <v>1</v>
-      </c>
-      <c r="I32" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="I32" t="n">
+        <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K32" t="n">
         <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="M32" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33"/>
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E33" t="n">
         <v>1</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="K33" t="n">
         <v>1</v>
       </c>
       <c r="L33" t="n">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="M33" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" t="n">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="B34" t="s">
+        <v>78</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G34" t="n">
         <v>1</v>
       </c>
       <c r="H34" t="n">
-        <v>1</v>
-      </c>
-      <c r="I34" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="K34" t="n">
         <v>1</v>
       </c>
       <c r="L34" t="n">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="M34" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35"/>
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>79</v>
+      </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E35" t="n">
         <v>1</v>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="n">
-        <v>1</v>
-      </c>
-      <c r="I35" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="K35" t="n">
         <v>1</v>
       </c>
       <c r="L35" t="n">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="M35" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" t="n">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="B36" t="s">
+        <v>81</v>
       </c>
       <c r="C36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H36" t="n">
         <v>1</v>
       </c>
-      <c r="I36" t="s">
-        <v>37</v>
+      <c r="I36" t="n">
+        <v>3</v>
       </c>
       <c r="J36" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K36" t="n">
         <v>1</v>
       </c>
       <c r="L36" t="n">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="M36" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" t="n">
-        <v>1</v>
+        <v>82</v>
+      </c>
+      <c r="B37" t="s">
+        <v>83</v>
       </c>
       <c r="C37" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G37" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H37" t="n">
         <v>1</v>
       </c>
-      <c r="I37" t="s">
-        <v>13</v>
+      <c r="I37" t="n">
+        <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K37" t="n">
         <v>1</v>
       </c>
       <c r="L37" t="n">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="M37" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" t="n">
-        <v>1</v>
+        <v>84</v>
+      </c>
+      <c r="B38" t="s">
+        <v>85</v>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38"/>
+        <v>2</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H38" t="n">
-        <v>1</v>
-      </c>
-      <c r="I38" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K38" t="n">
         <v>1</v>
       </c>
       <c r="L38" t="n">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="M38" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" t="n">
-        <v>1</v>
+        <v>86</v>
+      </c>
+      <c r="B39" t="s">
+        <v>87</v>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39"/>
+        <v>1</v>
+      </c>
+      <c r="G39" t="n">
+        <v>3</v>
+      </c>
       <c r="H39" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>3</v>
       </c>
       <c r="J39" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K39" t="n">
         <v>1</v>
       </c>
       <c r="L39" t="n">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="M39" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" t="n">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="B40" t="s">
+        <v>89</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H40" t="n">
         <v>1</v>
       </c>
-      <c r="I40" t="s">
-        <v>13</v>
+      <c r="I40" t="n">
+        <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K40" t="n">
         <v>1</v>
       </c>
       <c r="L40" t="n">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="M40" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41"/>
+        <v>90</v>
+      </c>
+      <c r="B41" t="s">
+        <v>91</v>
+      </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
         <v>1</v>
@@ -2041,215 +2405,241 @@
         <v>1</v>
       </c>
       <c r="H41" t="n">
-        <v>1</v>
-      </c>
-      <c r="I41" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="I41" t="n">
+        <v>3</v>
       </c>
       <c r="J41" t="s">
+        <v>15</v>
+      </c>
+      <c r="K41" t="n">
+        <v>1</v>
+      </c>
+      <c r="L41" t="n">
         <v>14</v>
       </c>
-      <c r="K41" t="n">
-        <v>1</v>
-      </c>
-      <c r="L41" t="n">
-        <v>4</v>
+      <c r="M41" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" t="n">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="B42" t="s">
+        <v>93</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G42" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H42" t="n">
         <v>1</v>
       </c>
-      <c r="I42" t="s">
-        <v>13</v>
+      <c r="I42" t="n">
+        <v>3</v>
       </c>
       <c r="J42" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K42" t="n">
         <v>1</v>
       </c>
       <c r="L42" t="n">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="M42" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>58</v>
-      </c>
-      <c r="B43" t="n">
-        <v>1</v>
+        <v>94</v>
+      </c>
+      <c r="B43" t="s">
+        <v>95</v>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" t="n">
-        <v>1</v>
-      </c>
-      <c r="H43"/>
-      <c r="I43" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="H43" t="n">
+        <v>3</v>
+      </c>
+      <c r="I43" t="n">
+        <v>3</v>
       </c>
       <c r="J43" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="K43" t="n">
         <v>1</v>
       </c>
       <c r="L43" t="n">
-        <v>5</v>
+        <v>18</v>
+      </c>
+      <c r="M43" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44"/>
+        <v>96</v>
+      </c>
+      <c r="B44" t="s">
+        <v>97</v>
+      </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44"/>
+        <v>1</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1</v>
+      </c>
       <c r="H44" t="n">
-        <v>1</v>
-      </c>
-      <c r="I44" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="I44" t="n">
+        <v>3</v>
       </c>
       <c r="J44" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K44" t="n">
         <v>1</v>
       </c>
       <c r="L44" t="n">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="M44" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" t="n">
-        <v>1</v>
+        <v>98</v>
+      </c>
+      <c r="B45" t="s">
+        <v>99</v>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F45" t="n">
         <v>1</v>
       </c>
       <c r="G45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H45" t="n">
         <v>1</v>
       </c>
-      <c r="I45" t="s">
-        <v>16</v>
+      <c r="I45" t="n">
+        <v>3</v>
       </c>
       <c r="J45" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K45" t="n">
         <v>1</v>
       </c>
       <c r="L45" t="n">
-        <v>6</v>
+        <v>17</v>
+      </c>
+      <c r="M45" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" t="n">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>101</v>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E46" t="n">
         <v>1</v>
       </c>
       <c r="F46" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G46" t="n">
         <v>1</v>
       </c>
       <c r="H46" t="n">
-        <v>1</v>
-      </c>
-      <c r="I46" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="I46" t="n">
+        <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K46" t="n">
         <v>1</v>
       </c>
       <c r="L46" t="n">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="M46" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>62</v>
-      </c>
-      <c r="B47" t="n">
-        <v>1</v>
-      </c>
-      <c r="C47"/>
+        <v>102</v>
+      </c>
+      <c r="B47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" t="n">
+        <v>3</v>
+      </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
         <v>1</v>
@@ -2263,31 +2653,34 @@
       <c r="H47" t="n">
         <v>1</v>
       </c>
-      <c r="I47" t="s">
-        <v>13</v>
+      <c r="I47" t="n">
+        <v>3</v>
       </c>
       <c r="J47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K47" t="n">
         <v>1</v>
       </c>
       <c r="L47" t="n">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="M47" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48" t="n">
-        <v>1</v>
+        <v>102</v>
+      </c>
+      <c r="B48" t="s">
+        <v>104</v>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" t="n">
         <v>1</v>
@@ -2301,31 +2694,34 @@
       <c r="H48" t="n">
         <v>1</v>
       </c>
-      <c r="I48" t="s">
-        <v>13</v>
+      <c r="I48" t="n">
+        <v>3</v>
       </c>
       <c r="J48" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K48" t="n">
         <v>1</v>
       </c>
       <c r="L48" t="n">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="M48" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>64</v>
-      </c>
-      <c r="B49" t="n">
-        <v>1</v>
+        <v>105</v>
+      </c>
+      <c r="B49" t="s">
+        <v>106</v>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" t="n">
         <v>1</v>
@@ -2334,33 +2730,36 @@
         <v>1</v>
       </c>
       <c r="G49" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H49" t="n">
-        <v>1</v>
-      </c>
-      <c r="I49" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="I49" t="n">
+        <v>3</v>
       </c>
       <c r="J49" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K49" t="n">
         <v>1</v>
       </c>
       <c r="L49" t="n">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="M49" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50" t="n">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="B50" t="s">
+        <v>108</v>
       </c>
       <c r="C50" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D50" t="n">
         <v>1</v>
@@ -2372,134 +2771,556 @@
         <v>1</v>
       </c>
       <c r="G50" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H50" t="n">
-        <v>1</v>
-      </c>
-      <c r="I50" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="I50" t="n">
+        <v>3</v>
       </c>
       <c r="J50" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K50" t="n">
         <v>1</v>
       </c>
       <c r="L50" t="n">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="M50" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>66</v>
-      </c>
-      <c r="B51" t="n">
-        <v>1</v>
+        <v>109</v>
+      </c>
+      <c r="B51" t="s">
+        <v>110</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E51" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F51" t="n">
         <v>1</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" t="n">
-        <v>1</v>
-      </c>
-      <c r="I51" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="I51" t="n">
+        <v>2</v>
       </c>
       <c r="J51" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K51" t="n">
         <v>1</v>
       </c>
       <c r="L51" t="n">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="M51" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>67</v>
-      </c>
-      <c r="B52"/>
+        <v>111</v>
+      </c>
+      <c r="B52" t="s">
+        <v>112</v>
+      </c>
       <c r="C52" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I52" t="s">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="I52" t="n">
+        <v>3</v>
       </c>
       <c r="J52" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K52" t="n">
         <v>1</v>
       </c>
       <c r="L52" t="n">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="M52" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>68</v>
-      </c>
-      <c r="B53" t="n">
-        <v>1</v>
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
+        <v>114</v>
       </c>
       <c r="C53" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H53" t="n">
-        <v>1</v>
-      </c>
-      <c r="I53" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="I53" t="n">
+        <v>3</v>
       </c>
       <c r="J53" t="s">
+        <v>19</v>
+      </c>
+      <c r="K53" t="n">
+        <v>1</v>
+      </c>
+      <c r="L53" t="n">
+        <v>18</v>
+      </c>
+      <c r="M53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" t="n">
+        <v>3</v>
+      </c>
+      <c r="D54" t="n">
+        <v>3</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1</v>
+      </c>
+      <c r="F54" t="n">
+        <v>3</v>
+      </c>
+      <c r="G54" t="n">
+        <v>3</v>
+      </c>
+      <c r="H54" t="n">
+        <v>3</v>
+      </c>
+      <c r="I54" t="n">
+        <v>3</v>
+      </c>
+      <c r="J54" t="s">
+        <v>15</v>
+      </c>
+      <c r="K54" t="n">
+        <v>1</v>
+      </c>
+      <c r="L54" t="n">
+        <v>20</v>
+      </c>
+      <c r="M54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>117</v>
+      </c>
+      <c r="B55" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" t="n">
+        <v>3</v>
+      </c>
+      <c r="D55" t="n">
+        <v>2</v>
+      </c>
+      <c r="E55" t="n">
+        <v>1</v>
+      </c>
+      <c r="F55" t="n">
+        <v>3</v>
+      </c>
+      <c r="G55" t="n">
+        <v>3</v>
+      </c>
+      <c r="H55" t="n">
+        <v>3</v>
+      </c>
+      <c r="I55" t="n">
+        <v>3</v>
+      </c>
+      <c r="J55" t="s">
+        <v>15</v>
+      </c>
+      <c r="K55" t="n">
+        <v>1</v>
+      </c>
+      <c r="L55" t="n">
+        <v>19</v>
+      </c>
+      <c r="M55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" t="n">
+        <v>3</v>
+      </c>
+      <c r="D56" t="n">
+        <v>3</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F56" t="n">
+        <v>3</v>
+      </c>
+      <c r="G56" t="n">
+        <v>3</v>
+      </c>
+      <c r="H56" t="n">
+        <v>3</v>
+      </c>
+      <c r="I56" t="n">
+        <v>3</v>
+      </c>
+      <c r="J56" t="s">
+        <v>15</v>
+      </c>
+      <c r="K56" t="n">
+        <v>1</v>
+      </c>
+      <c r="L56" t="n">
+        <v>20</v>
+      </c>
+      <c r="M56" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" t="n">
+        <v>3</v>
+      </c>
+      <c r="D57" t="n">
+        <v>3</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1</v>
+      </c>
+      <c r="F57" t="n">
+        <v>3</v>
+      </c>
+      <c r="G57" t="n">
+        <v>3</v>
+      </c>
+      <c r="H57" t="n">
+        <v>3</v>
+      </c>
+      <c r="I57" t="n">
+        <v>3</v>
+      </c>
+      <c r="J57" t="s">
+        <v>15</v>
+      </c>
+      <c r="K57" t="n">
+        <v>1</v>
+      </c>
+      <c r="L57" t="n">
+        <v>20</v>
+      </c>
+      <c r="M57" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" t="n">
+        <v>3</v>
+      </c>
+      <c r="D58" t="n">
+        <v>3</v>
+      </c>
+      <c r="E58" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" t="n">
+        <v>3</v>
+      </c>
+      <c r="G58" t="n">
+        <v>3</v>
+      </c>
+      <c r="H58" t="n">
+        <v>3</v>
+      </c>
+      <c r="I58" t="n">
+        <v>3</v>
+      </c>
+      <c r="J58" t="s">
+        <v>19</v>
+      </c>
+      <c r="K58" t="n">
+        <v>1</v>
+      </c>
+      <c r="L58" t="n">
+        <v>20</v>
+      </c>
+      <c r="M58" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" t="n">
+        <v>3</v>
+      </c>
+      <c r="D59" t="n">
+        <v>3</v>
+      </c>
+      <c r="E59" t="n">
+        <v>3</v>
+      </c>
+      <c r="F59" t="n">
+        <v>3</v>
+      </c>
+      <c r="G59" t="n">
+        <v>3</v>
+      </c>
+      <c r="H59" t="n">
+        <v>3</v>
+      </c>
+      <c r="I59" t="n">
+        <v>3</v>
+      </c>
+      <c r="J59" t="s">
+        <v>15</v>
+      </c>
+      <c r="K59" t="n">
+        <v>1</v>
+      </c>
+      <c r="L59" t="n">
+        <v>22</v>
+      </c>
+      <c r="M59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60" t="n">
+        <v>3</v>
+      </c>
+      <c r="D60" t="n">
+        <v>3</v>
+      </c>
+      <c r="E60" t="n">
+        <v>3</v>
+      </c>
+      <c r="F60" t="n">
+        <v>3</v>
+      </c>
+      <c r="G60" t="n">
+        <v>3</v>
+      </c>
+      <c r="H60" t="n">
+        <v>3</v>
+      </c>
+      <c r="I60" t="n">
+        <v>3</v>
+      </c>
+      <c r="J60" t="s">
+        <v>15</v>
+      </c>
+      <c r="K60" t="n">
+        <v>1</v>
+      </c>
+      <c r="L60" t="n">
+        <v>22</v>
+      </c>
+      <c r="M60" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>127</v>
+      </c>
+      <c r="B61" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" t="n">
+        <v>3</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" t="n">
+        <v>3</v>
+      </c>
+      <c r="G61" t="n">
+        <v>3</v>
+      </c>
+      <c r="H61" t="n">
+        <v>1</v>
+      </c>
+      <c r="I61" t="n">
+        <v>3</v>
+      </c>
+      <c r="J61" t="s">
+        <v>15</v>
+      </c>
+      <c r="K61" t="n">
+        <v>1</v>
+      </c>
+      <c r="L61" t="n">
+        <v>16</v>
+      </c>
+      <c r="M61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" t="s">
+        <v>130</v>
+      </c>
+      <c r="C62"/>
+      <c r="D62" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" t="n">
+        <v>1</v>
+      </c>
+      <c r="F62" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" t="n">
+        <v>1</v>
+      </c>
+      <c r="I62" t="n">
+        <v>3</v>
+      </c>
+      <c r="J62" t="s">
+        <v>19</v>
+      </c>
+      <c r="K62" t="n">
+        <v>1</v>
+      </c>
+      <c r="L62" t="n">
+        <v>9</v>
+      </c>
+      <c r="M62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>131</v>
+      </c>
+      <c r="B63" t="s">
+        <v>132</v>
+      </c>
+      <c r="C63" t="n">
+        <v>3</v>
+      </c>
+      <c r="D63" t="n">
+        <v>3</v>
+      </c>
+      <c r="E63" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" t="n">
+        <v>1</v>
+      </c>
+      <c r="I63" t="n">
+        <v>3</v>
+      </c>
+      <c r="J63" t="s">
+        <v>15</v>
+      </c>
+      <c r="K63" t="n">
+        <v>1</v>
+      </c>
+      <c r="L63" t="n">
         <v>14</v>
       </c>
-      <c r="K53" t="n">
-        <v>1</v>
-      </c>
-      <c r="L53" t="n">
-        <v>4</v>
+      <c r="M63" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>